<commit_message>
Add charts to benchmark
</commit_message>
<xml_diff>
--- a/doc/benchmark/00 Instance generator benchmark.xlsx
+++ b/doc/benchmark/00 Instance generator benchmark.xlsx
@@ -1,34 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\TSP-con-pick-up-and-delivery\doc\benchmark\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29DACFD-9499-41C8-B05D-A867737AD4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Generazione delle istanze da R = 2 a R = 30</t>
+  </si>
+  <si>
+    <t>Numero di richieste</t>
+  </si>
+  <si>
+    <t>Durata (in secondi)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,81 +72,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,271 +380,270 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Generazione delle istanze da R = 2 a R = 30</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Numero di richieste</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Durata (in secondi)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.02014350006356835</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.014350006356835E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.004825899843126535</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+      <c r="B4" s="1">
+        <v>4.8258998431265354E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
-        <v>0.008209200110286474</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
+      <c r="B5" s="1">
+        <v>8.2092001102864742E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
-        <v>0.02659159991890192</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+      <c r="B6" s="1">
+        <v>2.659159991890192E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.04932689992710948</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="B7" s="1">
+        <v>4.932689992710948E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
-        <v>0.03386600012890995</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
+      <c r="B8" s="1">
+        <v>3.3866000128909952E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
-        <v>0.06050460017286241</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
+      <c r="B9" s="1">
+        <v>6.0504600172862411E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.05890910001471639</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
+      <c r="B10" s="1">
+        <v>5.8909100014716387E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.08677819999866188</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
+      <c r="B11" s="1">
+        <v>8.6778199998661876E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
-        <v>0.115321199875325</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
+      <c r="B12" s="1">
+        <v>0.11532119987532501</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
-        <v>0.08851619996130466</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
+      <c r="B13" s="1">
+        <v>8.8516199961304665E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" s="1">
         <v>0.1158380000852048</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
-        <v>0.1123685000929981</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
+      <c r="B15" s="1">
+        <v>0.11236850009299811</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" s="1">
         <v>0.1123519001994282</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="n">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
-        <v>0.1203799000941217</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
+      <c r="B17" s="1">
+        <v>0.12037990009412169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" t="n">
-        <v>0.1296732001937926</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
+      <c r="B18" s="1">
+        <v>0.12967320019379261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" s="1">
         <v>0.1336841001175344</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="n">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" s="1">
         <v>0.1294644000008702</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="n">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" s="1">
         <v>0.1513370999600738</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="n">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22" s="1">
         <v>0.1626541998703033</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="n">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" t="n">
-        <v>0.1747681000269949</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
+      <c r="B23" s="1">
+        <v>0.17476810002699489</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24" s="1">
         <v>0.1854369000066072</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="n">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" s="1">
         <v>0.1969628999941051</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="n">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" t="n">
-        <v>0.2315903000999242</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
+      <c r="B26" s="1">
+        <v>0.23159030009992421</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" t="n">
-        <v>0.2229019000660628</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
+      <c r="B27" s="1">
+        <v>0.22290190006606281</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" t="n">
-        <v>0.2379040999803692</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
+      <c r="B28" s="1">
+        <v>0.23790409998036921</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" t="n">
-        <v>0.2737943001557142</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
+      <c r="B29" s="1">
+        <v>0.27379430015571421</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" t="n">
-        <v>0.2594697999302298</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
+      <c r="B30" s="1">
+        <v>0.25946979993022978</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" t="n">
-        <v>0.2743644001893699</v>
+      <c r="B31" s="1">
+        <v>0.27436440018936992</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>